<commit_message>
feature/GDE-9262 addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A239E1D-4518-45B6-B701-53B45A164CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FBB791-636B-4837-9FA6-6166AC3FCB07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="560">
   <si>
     <t>rowid</t>
   </si>
@@ -431,9 +431,6 @@
     <t>RemittanceInstruction_RTGSDescriptionAUDPrefix2</t>
   </si>
   <si>
-    <t>RemittanceInstruction_DDADescriptionAUD</t>
-  </si>
-  <si>
     <t>RemittanceInstruction_DDADescriptionAUD2</t>
   </si>
   <si>
@@ -525,18 +522,6 @@
   </si>
   <si>
     <t>RemittanceInstruction_MethodType</t>
-  </si>
-  <si>
-    <t>RemittanceInstruction_DDAMethod</t>
-  </si>
-  <si>
-    <t>RemittanceInstruction_DDAAccountName</t>
-  </si>
-  <si>
-    <t>RemittanceInstruction_DDAAccountNumber</t>
-  </si>
-  <si>
-    <t>RemittanceInstruction_DDACurrencyAUD</t>
   </si>
   <si>
     <t>RemittanceInstruction_DDACurrencyUSD</t>
@@ -724,9 +709,6 @@
     <t>RI_SendersCorrespondent_Checkbox</t>
   </si>
   <si>
-    <t>Remittance_Instruction</t>
-  </si>
-  <si>
     <t>NoticesSummary</t>
   </si>
   <si>
@@ -1711,6 +1693,21 @@
   </si>
   <si>
     <t>1 Months</t>
+  </si>
+  <si>
+    <t>RemittanceInstruction_Method</t>
+  </si>
+  <si>
+    <t>RemittanceInstruction_AccountName</t>
+  </si>
+  <si>
+    <t>RemittanceInstruction_AccountNumber</t>
+  </si>
+  <si>
+    <t>RemittanceInstruction_Currency</t>
+  </si>
+  <si>
+    <t>Remittance_Description</t>
   </si>
 </sst>
 </file>
@@ -1896,7 +1893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1959,7 +1956,6 @@
     <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1980,6 +1976,8 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2660,16 +2658,16 @@
       <c r="A2" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="45" t="s">
         <v>85</v>
       </c>
       <c r="F2" s="15" t="s">
@@ -2746,10 +2744,10 @@
       <c r="AG2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="AH2" s="46" t="s">
+      <c r="AH2" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="AI2" s="46" t="s">
+      <c r="AI2" s="45" t="s">
         <v>90</v>
       </c>
       <c r="AJ2" s="11"/>
@@ -2800,29 +2798,29 @@
       <c r="CC2" s="10"/>
       <c r="CD2" s="10"/>
       <c r="CE2" s="10"/>
-      <c r="CF2" s="46"/>
-      <c r="CG2" s="46"/>
-      <c r="CH2" s="46"/>
-      <c r="CI2" s="46"/>
-      <c r="CJ2" s="46"/>
-      <c r="CK2" s="46"/>
-      <c r="CL2" s="46"/>
-      <c r="CM2" s="46"/>
-      <c r="CN2" s="46"/>
-      <c r="CO2" s="46"/>
-      <c r="CP2" s="46"/>
-      <c r="CQ2" s="46"/>
-      <c r="CR2" s="46"/>
-      <c r="CS2" s="46"/>
-      <c r="CT2" s="46"/>
-      <c r="CU2" s="46"/>
-      <c r="CV2" s="46"/>
-      <c r="CW2" s="46"/>
-      <c r="CX2" s="46"/>
-      <c r="CY2" s="46"/>
-      <c r="CZ2" s="46"/>
-      <c r="DA2" s="46"/>
-      <c r="DB2" s="46"/>
+      <c r="CF2" s="45"/>
+      <c r="CG2" s="45"/>
+      <c r="CH2" s="45"/>
+      <c r="CI2" s="45"/>
+      <c r="CJ2" s="45"/>
+      <c r="CK2" s="45"/>
+      <c r="CL2" s="45"/>
+      <c r="CM2" s="45"/>
+      <c r="CN2" s="45"/>
+      <c r="CO2" s="45"/>
+      <c r="CP2" s="45"/>
+      <c r="CQ2" s="45"/>
+      <c r="CR2" s="45"/>
+      <c r="CS2" s="45"/>
+      <c r="CT2" s="45"/>
+      <c r="CU2" s="45"/>
+      <c r="CV2" s="45"/>
+      <c r="CW2" s="45"/>
+      <c r="CX2" s="45"/>
+      <c r="CY2" s="45"/>
+      <c r="CZ2" s="45"/>
+      <c r="DA2" s="45"/>
+      <c r="DB2" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2835,10 +2833,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:EF2"/>
+  <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BD13" sqref="BD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2897,8 +2895,7 @@
     <col min="53" max="53" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="19" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="21" bestFit="1" customWidth="1"/>
@@ -2908,94 +2905,89 @@
     <col min="64" max="64" width="28" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="25" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="40" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="24" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="24" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="102" max="103" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="19" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="98" max="99" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="19" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="21" bestFit="1" customWidth="1"/>
     <col min="108" max="108" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="21" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="19" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="19" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="20" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="19" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="19" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="20" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:136" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:135" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="44" t="s">
         <v>102</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>105</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3032,7 +3024,7 @@
         <v>116</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>117</v>
@@ -3172,625 +3164,619 @@
       <c r="BL1" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BM1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="BN1" s="6" t="s">
+      <c r="BN1" s="2" t="s">
         <v>164</v>
       </c>
       <c r="BO1" s="2" t="s">
         <v>165</v>
       </c>
       <c r="BP1" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="BU1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="CA1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="CB1" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="CC1" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="CD1" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="BZ1" s="2" t="s">
+      <c r="CE1" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="CA1" s="2" t="s">
+      <c r="CF1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="CB1" s="2" t="s">
+      <c r="CG1" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="CC1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="CD1" s="2" t="s">
+      <c r="CI1" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="CE1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="CF1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CL1" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="CH1" s="2" t="s">
+      <c r="CM1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="CJ1" s="2" t="s">
+      <c r="CO1" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="CK1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="CL1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="CM1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="CN1" s="2" t="s">
+      <c r="CS1" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="CO1" s="2" t="s">
+      <c r="CT1" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="CP1" s="2" t="s">
+      <c r="CU1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="CQ1" s="2" t="s">
+      <c r="CV1" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="CR1" s="2" t="s">
+      <c r="CW1" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="CS1" s="2" t="s">
+      <c r="CX1" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="CT1" s="2" t="s">
+      <c r="CY1" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="CU1" s="2" t="s">
+      <c r="CZ1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="CV1" s="2" t="s">
+      <c r="DA1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="CW1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="CX1" s="2" t="s">
+      <c r="DC1" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="CY1" s="2" t="s">
+      <c r="DD1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DE1" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="DA1" s="2" t="s">
+      <c r="DF1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="DB1" s="2" t="s">
+      <c r="DG1" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="DC1" s="2" t="s">
+      <c r="DH1" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="DD1" s="2" t="s">
+      <c r="DI1" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="DE1" s="2" t="s">
+      <c r="DJ1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="DF1" s="2" t="s">
+      <c r="DK1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="DG1" s="2" t="s">
+      <c r="DL1" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="DH1" s="2" t="s">
+      <c r="DM1" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="DI1" s="5" t="s">
+      <c r="DN1" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="DJ1" s="2" t="s">
+      <c r="DO1" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="DK1" s="2" t="s">
+      <c r="DP1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="DL1" s="2" t="s">
+      <c r="DQ1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="DM1" s="2" t="s">
+      <c r="DR1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="DN1" s="2" t="s">
+      <c r="DS1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="DO1" s="2" t="s">
+      <c r="DT1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="DP1" s="2" t="s">
+      <c r="DU1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="DQ1" s="2" t="s">
+      <c r="DV1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="DR1" s="2" t="s">
+      <c r="DW1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="DS1" s="2" t="s">
+      <c r="DX1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="DT1" s="2" t="s">
+      <c r="DY1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="DU1" s="2" t="s">
+      <c r="DZ1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="DV1" s="2" t="s">
+      <c r="EA1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="DW1" s="2" t="s">
+      <c r="EB1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="DX1" s="2" t="s">
+      <c r="EC1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="DY1" s="2" t="s">
+      <c r="ED1" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="DZ1" s="2" t="s">
+      <c r="EE1" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="EA1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:135" s="20" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="EB1" s="2" t="s">
+      <c r="C2" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="EC1" s="2" t="s">
+      <c r="D2" s="38" t="s">
         <v>231</v>
-      </c>
-      <c r="ED1" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="EE1" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="EF1" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="2" spans="1:136" s="20" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>236</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>237</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="38" t="s">
+        <v>232</v>
+      </c>
+      <c r="G2" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="L2" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="38" t="s">
+      <c r="M2" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="N2" s="39" t="s">
         <v>240</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="O2" s="39" t="s">
         <v>241</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="P2" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="Q2" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="L2" s="37" t="s">
+      <c r="R2" s="45" t="s">
+        <v>418</v>
+      </c>
+      <c r="S2" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="M2" s="37" t="s">
+      <c r="T2" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="U2" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="V2" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="W2" s="40" t="s">
         <v>248</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="X2" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y2" s="42" t="s">
         <v>249</v>
       </c>
-      <c r="R2" s="46" t="s">
-        <v>424</v>
-      </c>
-      <c r="S2" s="41" t="s">
+      <c r="Z2" s="42" t="s">
         <v>250</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="AA2" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="AB2" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC2" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="AD2" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="AE2" s="56" t="s">
         <v>252</v>
       </c>
-      <c r="V2" s="37" t="s">
+      <c r="AF2" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="W2" s="40" t="s">
+      <c r="AG2" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="X2" s="41" t="s">
-        <v>248</v>
-      </c>
-      <c r="Y2" s="42" t="s">
+      <c r="AH2" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="Z2" s="42" t="s">
+      <c r="AI2" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="AA2" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="AB2" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="AC2" s="42" t="s">
-        <v>256</v>
-      </c>
-      <c r="AD2" s="37" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="AE2" s="44" t="s">
-        <v>258</v>
-      </c>
-      <c r="AF2" s="46" t="s">
+      <c r="AK2" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AL2" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="AH2" s="46" t="s">
+      <c r="AM2" s="57" t="s">
         <v>261</v>
       </c>
-      <c r="AI2" s="46" t="s">
+      <c r="AN2" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="AJ2" s="46" t="s">
+      <c r="AO2" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="AK2" s="46" t="s">
+      <c r="AP2" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="AL2" s="46" t="s">
+      <c r="AQ2" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="AM2" s="46" t="s">
+      <c r="AR2" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="AN2" s="16" t="s">
-        <v>267</v>
-      </c>
-      <c r="AO2" s="46" t="s">
-        <v>268</v>
-      </c>
-      <c r="AP2" s="46" t="s">
-        <v>269</v>
-      </c>
-      <c r="AQ2" s="46" t="s">
-        <v>270</v>
-      </c>
-      <c r="AR2" s="46" t="s">
-        <v>271</v>
-      </c>
-      <c r="AS2" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="AT2" s="37" t="s">
+      <c r="AS2" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="AU2" s="16"/>
+      <c r="AT2" s="16"/>
+      <c r="AU2" s="16" t="s">
+        <v>96</v>
+      </c>
       <c r="AV2" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="AW2" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="AX2" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AY2" s="7" t="s">
+      <c r="AX2" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="AY2" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="AZ2" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA2" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="BB2" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="BC2" s="43" t="s">
+        <v>272</v>
+      </c>
+      <c r="BD2" s="43" t="s">
         <v>273</v>
       </c>
-      <c r="AZ2" s="16" t="s">
+      <c r="BE2" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="BA2" s="37" t="s">
+      <c r="BF2" s="16" t="s">
         <v>275</v>
       </c>
-      <c r="BB2" s="16" t="s">
+      <c r="BG2" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="BC2" s="16" t="s">
+      <c r="BH2" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="BI2" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="BD2" s="43" t="s">
+      <c r="BJ2" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="BE2" s="43" t="s">
+      <c r="BK2" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="BL2" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="BM2" s="16" t="s">
         <v>279</v>
       </c>
-      <c r="BF2" s="16" t="s">
+      <c r="BN2" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="BG2" s="16" t="s">
+      <c r="BO2" s="57" t="s">
         <v>281</v>
       </c>
-      <c r="BH2" s="16" t="s">
+      <c r="BP2" s="38" t="s">
+        <v>258</v>
+      </c>
+      <c r="BQ2" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="BI2" s="16" t="s">
+      <c r="BR2" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="BS2" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="BT2" s="42" t="s">
+        <v>264</v>
+      </c>
+      <c r="BU2" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="BV2" s="43" t="s">
+        <v>286</v>
+      </c>
+      <c r="BW2" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="BX2" s="43" t="s">
+        <v>288</v>
+      </c>
+      <c r="BY2" s="43" t="s">
+        <v>289</v>
+      </c>
+      <c r="BZ2" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="CA2" s="52" t="s">
+        <v>291</v>
+      </c>
+      <c r="CB2" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="CC2" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="CD2" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="CE2" s="51" t="s">
+        <v>294</v>
+      </c>
+      <c r="CF2" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="CG2" s="51" t="s">
+        <v>285</v>
+      </c>
+      <c r="CH2" s="43" t="s">
+        <v>295</v>
+      </c>
+      <c r="CI2" s="43" t="s">
+        <v>296</v>
+      </c>
+      <c r="CJ2" s="43" t="s">
+        <v>297</v>
+      </c>
+      <c r="CK2" s="43" t="s">
         <v>280</v>
       </c>
-      <c r="BJ2" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="BK2" s="16" t="s">
-        <v>284</v>
-      </c>
-      <c r="BL2" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="BM2" s="37" t="s">
+      <c r="CL2" s="43" t="s">
+        <v>287</v>
+      </c>
+      <c r="CM2" s="43" t="s">
+        <v>298</v>
+      </c>
+      <c r="CN2" s="43" t="s">
+        <v>299</v>
+      </c>
+      <c r="CO2" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="CP2" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="CQ2" s="43" t="s">
+        <v>302</v>
+      </c>
+      <c r="CR2" s="43" t="s">
+        <v>303</v>
+      </c>
+      <c r="CS2" s="43" t="s">
+        <v>304</v>
+      </c>
+      <c r="CT2" s="43" t="s">
+        <v>305</v>
+      </c>
+      <c r="CU2" s="43" t="s">
+        <v>306</v>
+      </c>
+      <c r="CV2" s="43" t="s">
+        <v>307</v>
+      </c>
+      <c r="CW2" s="43" t="s">
+        <v>251</v>
+      </c>
+      <c r="CX2" s="43" t="s">
+        <v>308</v>
+      </c>
+      <c r="CY2" s="43" t="s">
+        <v>309</v>
+      </c>
+      <c r="CZ2" s="53" t="s">
+        <v>310</v>
+      </c>
+      <c r="DA2" s="43" t="s">
+        <v>311</v>
+      </c>
+      <c r="DB2" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="DC2" s="51" t="s">
+        <v>293</v>
+      </c>
+      <c r="DD2" s="51" t="s">
+        <v>311</v>
+      </c>
+      <c r="DE2" s="51" t="s">
+        <v>313</v>
+      </c>
+      <c r="DF2" s="51"/>
+      <c r="DG2" s="51"/>
+      <c r="DH2" s="51" t="s">
+        <v>314</v>
+      </c>
+      <c r="DI2" s="51" t="s">
+        <v>312</v>
+      </c>
+      <c r="DJ2" s="51" t="s">
+        <v>315</v>
+      </c>
+      <c r="DK2" s="51" t="s">
+        <v>316</v>
+      </c>
+      <c r="DL2" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="DM2" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="DN2" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="DO2" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="DP2" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="DQ2" s="54" t="s">
+        <v>321</v>
+      </c>
+      <c r="DR2" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="DS2" s="51" t="s">
         <v>250</v>
       </c>
-      <c r="BN2" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="BO2" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="BP2" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="BQ2" s="37" t="s">
-        <v>288</v>
-      </c>
-      <c r="BR2" s="41" t="s">
-        <v>289</v>
-      </c>
-      <c r="BS2" s="42" t="s">
-        <v>290</v>
-      </c>
-      <c r="BT2" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="BU2" s="52" t="s">
-        <v>291</v>
-      </c>
-      <c r="BV2" s="43" t="s">
-        <v>292</v>
-      </c>
-      <c r="BW2" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="BX2" s="43" t="s">
-        <v>294</v>
-      </c>
-      <c r="BY2" s="43" t="s">
-        <v>295</v>
-      </c>
-      <c r="BZ2" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="CA2" s="53" t="s">
-        <v>297</v>
-      </c>
-      <c r="CB2" s="52" t="s">
-        <v>291</v>
-      </c>
-      <c r="CC2" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="CD2" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="CE2" s="52" t="s">
-        <v>300</v>
-      </c>
-      <c r="CF2" s="52" t="s">
-        <v>270</v>
-      </c>
-      <c r="CG2" s="52" t="s">
-        <v>291</v>
-      </c>
-      <c r="CH2" s="43" t="s">
-        <v>301</v>
-      </c>
-      <c r="CI2" s="43" t="s">
-        <v>302</v>
-      </c>
-      <c r="CJ2" s="43" t="s">
-        <v>303</v>
-      </c>
-      <c r="CK2" s="43" t="s">
-        <v>286</v>
-      </c>
-      <c r="CL2" s="43" t="s">
-        <v>293</v>
-      </c>
-      <c r="CM2" s="43" t="s">
-        <v>304</v>
-      </c>
-      <c r="CN2" s="43" t="s">
-        <v>305</v>
-      </c>
-      <c r="CO2" s="43" t="s">
-        <v>306</v>
-      </c>
-      <c r="CP2" s="43" t="s">
-        <v>307</v>
-      </c>
-      <c r="CQ2" s="43" t="s">
-        <v>308</v>
-      </c>
-      <c r="CR2" s="43" t="s">
-        <v>309</v>
-      </c>
-      <c r="CS2" s="43" t="s">
-        <v>310</v>
-      </c>
-      <c r="CT2" s="43" t="s">
-        <v>311</v>
-      </c>
-      <c r="CU2" s="43" t="s">
-        <v>312</v>
-      </c>
-      <c r="CV2" s="43" t="s">
-        <v>313</v>
-      </c>
-      <c r="CW2" s="43" t="s">
-        <v>257</v>
-      </c>
-      <c r="CX2" s="43" t="s">
-        <v>314</v>
-      </c>
-      <c r="CY2" s="43" t="s">
-        <v>315</v>
-      </c>
-      <c r="CZ2" s="54" t="s">
-        <v>316</v>
-      </c>
-      <c r="DA2" s="43" t="s">
-        <v>317</v>
-      </c>
-      <c r="DB2" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="DC2" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="DD2" s="52" t="s">
-        <v>317</v>
-      </c>
-      <c r="DE2" s="52" t="s">
-        <v>319</v>
-      </c>
-      <c r="DF2" s="52"/>
-      <c r="DG2" s="52"/>
-      <c r="DH2" s="52" t="s">
-        <v>320</v>
-      </c>
-      <c r="DI2" s="52" t="s">
-        <v>318</v>
-      </c>
-      <c r="DJ2" s="52" t="s">
-        <v>321</v>
-      </c>
-      <c r="DK2" s="52" t="s">
+      <c r="DT2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="DU2" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="DV2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="DW2" s="51" t="s">
+        <v>249</v>
+      </c>
+      <c r="DX2" s="51" t="s">
         <v>322</v>
       </c>
-      <c r="DL2" s="52" t="s">
-        <v>323</v>
-      </c>
-      <c r="DM2" s="52" t="s">
+      <c r="DY2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="DZ2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="EA2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="EB2" s="51" t="s">
+        <v>322</v>
+      </c>
+      <c r="EC2" s="51" t="s">
+        <v>250</v>
+      </c>
+      <c r="ED2" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="DN2" s="52" t="s">
-        <v>323</v>
-      </c>
-      <c r="DO2" s="52" t="s">
+      <c r="EE2" s="55" t="s">
         <v>325</v>
-      </c>
-      <c r="DP2" s="52" t="s">
-        <v>326</v>
-      </c>
-      <c r="DQ2" s="55" t="s">
-        <v>327</v>
-      </c>
-      <c r="DR2" s="52" t="s">
-        <v>326</v>
-      </c>
-      <c r="DS2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="DT2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="DU2" s="52" t="s">
-        <v>255</v>
-      </c>
-      <c r="DV2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="DW2" s="52" t="s">
-        <v>255</v>
-      </c>
-      <c r="DX2" s="52" t="s">
-        <v>328</v>
-      </c>
-      <c r="DY2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="DZ2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="EA2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="EB2" s="52" t="s">
-        <v>328</v>
-      </c>
-      <c r="EC2" s="52" t="s">
-        <v>256</v>
-      </c>
-      <c r="ED2" s="52" t="s">
-        <v>329</v>
-      </c>
-      <c r="EE2" s="56" t="s">
-        <v>330</v>
-      </c>
-      <c r="EF2" s="56" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3912,536 +3898,536 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="J1" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="K1" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="L1" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="M1" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="P1" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="BB1" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="BC1" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="BD1" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="BE1" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="BA1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="BB1" s="3" t="s">
+      <c r="BH1" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="BC1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="BD1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="BG1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CL1" s="3" t="s">
         <v>413</v>
-      </c>
-      <c r="CG1" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="CH1" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="CI1" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="CJ1" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="CK1" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="CL1" s="3" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:90" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>416</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45" t="s">
+        <v>264</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" s="45" t="s">
+        <v>322</v>
+      </c>
+      <c r="M2" s="45" t="s">
+        <v>418</v>
+      </c>
+      <c r="N2" s="50" t="s">
+        <v>419</v>
+      </c>
+      <c r="O2" s="50" t="s">
+        <v>420</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="S2" s="46" t="s">
+        <v>423</v>
+      </c>
+      <c r="T2" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="U2" s="47" t="s">
+        <v>424</v>
+      </c>
+      <c r="V2" s="47" t="s">
+        <v>424</v>
+      </c>
+      <c r="W2" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="X2" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="Y2" s="45" t="s">
+        <v>426</v>
+      </c>
+      <c r="Z2" s="45" t="s">
+        <v>427</v>
+      </c>
+      <c r="AA2" s="39" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>420</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>421</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>422</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>423</v>
-      </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46" t="s">
-        <v>270</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="46" t="s">
-        <v>238</v>
-      </c>
-      <c r="K2" s="46" t="s">
-        <v>245</v>
-      </c>
-      <c r="L2" s="46" t="s">
-        <v>328</v>
-      </c>
-      <c r="M2" s="46" t="s">
-        <v>424</v>
-      </c>
-      <c r="N2" s="51" t="s">
-        <v>425</v>
-      </c>
-      <c r="O2" s="51" t="s">
-        <v>426</v>
-      </c>
-      <c r="P2" s="46" t="s">
-        <v>427</v>
-      </c>
-      <c r="Q2" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="S2" s="47" t="s">
-        <v>429</v>
-      </c>
-      <c r="T2" s="48" t="s">
-        <v>282</v>
-      </c>
-      <c r="U2" s="48" t="s">
+      <c r="AF2" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="AG2" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="AH2" s="45" t="s">
         <v>430</v>
       </c>
-      <c r="V2" s="48" t="s">
-        <v>430</v>
-      </c>
-      <c r="W2" s="47" t="s">
+      <c r="AI2" s="45" t="s">
         <v>431</v>
       </c>
-      <c r="X2" s="47" t="s">
-        <v>427</v>
-      </c>
-      <c r="Y2" s="46" t="s">
+      <c r="AJ2" s="45" t="s">
         <v>432</v>
       </c>
-      <c r="Z2" s="46" t="s">
+      <c r="AK2" s="45" t="s">
+        <v>432</v>
+      </c>
+      <c r="AL2" s="50" t="s">
         <v>433</v>
       </c>
-      <c r="AA2" s="39" t="s">
+      <c r="AM2" s="50" t="s">
         <v>434</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AN2" s="50" t="s">
         <v>435</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AO2" s="50" t="s">
         <v>435</v>
       </c>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="AF2" s="46" t="s">
-        <v>277</v>
-      </c>
-      <c r="AG2" s="46" t="s">
-        <v>240</v>
-      </c>
-      <c r="AH2" s="46" t="s">
+      <c r="AP2" s="50" t="s">
         <v>436</v>
       </c>
-      <c r="AI2" s="46" t="s">
+      <c r="AQ2" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="AJ2" s="46" t="s">
+      <c r="AR2" s="50" t="s">
         <v>438</v>
       </c>
-      <c r="AK2" s="46" t="s">
-        <v>438</v>
-      </c>
-      <c r="AL2" s="51" t="s">
+      <c r="AS2" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="AT2" s="50" t="s">
+        <v>250</v>
+      </c>
+      <c r="AU2" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="AM2" s="51" t="s">
+      <c r="AV2" s="50" t="s">
         <v>440</v>
       </c>
-      <c r="AN2" s="51" t="s">
+      <c r="AW2" s="50" t="s">
         <v>441</v>
       </c>
-      <c r="AO2" s="51" t="s">
-        <v>441</v>
-      </c>
-      <c r="AP2" s="51" t="s">
+      <c r="AX2" s="49" t="s">
         <v>442</v>
       </c>
-      <c r="AQ2" s="51" t="s">
+      <c r="AY2" s="49" t="s">
         <v>443</v>
       </c>
-      <c r="AR2" s="51" t="s">
+      <c r="AZ2" s="50" t="s">
         <v>444</v>
       </c>
-      <c r="AS2" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="AT2" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="AU2" s="51" t="s">
+      <c r="BA2" s="50" t="s">
+        <v>437</v>
+      </c>
+      <c r="BB2" s="50" t="s">
+        <v>435</v>
+      </c>
+      <c r="BC2" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="AV2" s="51" t="s">
+      <c r="BD2" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="AW2" s="51" t="s">
+      <c r="BE2" s="33" t="s">
         <v>447</v>
       </c>
-      <c r="AX2" s="50" t="s">
+      <c r="BF2" s="31" t="s">
         <v>448</v>
       </c>
-      <c r="AY2" s="50" t="s">
-        <v>449</v>
-      </c>
-      <c r="AZ2" s="51" t="s">
-        <v>450</v>
-      </c>
-      <c r="BA2" s="51" t="s">
-        <v>443</v>
-      </c>
-      <c r="BB2" s="51" t="s">
-        <v>441</v>
-      </c>
-      <c r="BC2" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="BD2" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="BE2" s="33" t="s">
-        <v>453</v>
-      </c>
-      <c r="BF2" s="31" t="s">
-        <v>454</v>
-      </c>
       <c r="BG2" s="31" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="BH2" s="31" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="BI2" s="31" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="BJ2" s="31" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BK2" s="31" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BL2" s="31" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BM2" s="31" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BN2" s="31" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="BO2" s="31"/>
       <c r="BP2" s="31" t="s">
+        <v>423</v>
+      </c>
+      <c r="BQ2" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="BR2" s="31" t="s">
+        <v>425</v>
+      </c>
+      <c r="BS2" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="BT2" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="BU2" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="BV2" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="BW2" s="31" t="s">
+        <v>452</v>
+      </c>
+      <c r="BX2" s="31" t="s">
+        <v>453</v>
+      </c>
+      <c r="BY2" s="31" t="s">
+        <v>454</v>
+      </c>
+      <c r="BZ2" s="31" t="s">
+        <v>455</v>
+      </c>
+      <c r="CA2" s="31" t="s">
+        <v>456</v>
+      </c>
+      <c r="CB2" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="CC2" s="31" t="s">
+        <v>423</v>
+      </c>
+      <c r="CD2" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="CE2" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="CF2" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="CG2" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="CH2" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="CI2" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="CJ2" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="CK2" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="CL2" s="31" t="s">
         <v>429</v>
-      </c>
-      <c r="BQ2" s="31" t="s">
-        <v>455</v>
-      </c>
-      <c r="BR2" s="31" t="s">
-        <v>431</v>
-      </c>
-      <c r="BS2" s="31" t="s">
-        <v>329</v>
-      </c>
-      <c r="BT2" s="31" t="s">
-        <v>455</v>
-      </c>
-      <c r="BU2" s="31" t="s">
-        <v>456</v>
-      </c>
-      <c r="BV2" s="31" t="s">
-        <v>457</v>
-      </c>
-      <c r="BW2" s="31" t="s">
-        <v>458</v>
-      </c>
-      <c r="BX2" s="31" t="s">
-        <v>459</v>
-      </c>
-      <c r="BY2" s="31" t="s">
-        <v>460</v>
-      </c>
-      <c r="BZ2" s="31" t="s">
-        <v>461</v>
-      </c>
-      <c r="CA2" s="31" t="s">
-        <v>462</v>
-      </c>
-      <c r="CB2" s="31" t="s">
-        <v>463</v>
-      </c>
-      <c r="CC2" s="31" t="s">
-        <v>429</v>
-      </c>
-      <c r="CD2" s="31" t="s">
-        <v>282</v>
-      </c>
-      <c r="CE2" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="CF2" s="31" t="s">
-        <v>307</v>
-      </c>
-      <c r="CG2" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="CH2" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="CI2" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="CJ2" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="CK2" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="CL2" s="31" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="AN7" s="49"/>
+      <c r="AN7" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4502,127 +4488,127 @@
         <v>1</v>
       </c>
       <c r="C1" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>465</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>466</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>334</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>336</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>337</v>
-      </c>
-      <c r="G1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>471</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>472</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>474</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="Q1" s="25" t="s">
         <v>475</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>477</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>479</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="W1" s="26" t="s">
         <v>481</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>482</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="Y1" s="25" t="s">
         <v>483</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="Z1" s="25" t="s">
         <v>484</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="AA1" s="25" t="s">
         <v>485</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="AB1" s="25" t="s">
         <v>486</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="AC1" s="25" t="s">
         <v>487</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>488</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="AE1" s="25" t="s">
         <v>489</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="AF1" s="25" t="s">
         <v>490</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AG1" s="25" t="s">
         <v>491</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AH1" s="25" t="s">
         <v>492</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AI1" s="25" t="s">
         <v>493</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AJ1" s="25" t="s">
         <v>494</v>
       </c>
-      <c r="AE1" s="25" t="s">
+      <c r="AK1" s="25" t="s">
         <v>495</v>
       </c>
-      <c r="AF1" s="25" t="s">
+      <c r="AL1" s="25" t="s">
         <v>496</v>
       </c>
-      <c r="AG1" s="25" t="s">
+      <c r="AM1" s="25" t="s">
         <v>497</v>
       </c>
-      <c r="AH1" s="25" t="s">
+      <c r="AN1" s="25" t="s">
         <v>498</v>
       </c>
-      <c r="AI1" s="25" t="s">
+      <c r="AO1" s="25" t="s">
         <v>499</v>
       </c>
-      <c r="AJ1" s="25" t="s">
+      <c r="AP1" s="25" t="s">
         <v>500</v>
       </c>
-      <c r="AK1" s="25" t="s">
+      <c r="AQ1" s="25" t="s">
         <v>501</v>
-      </c>
-      <c r="AL1" s="25" t="s">
-        <v>502</v>
-      </c>
-      <c r="AM1" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="AN1" s="25" t="s">
-        <v>504</v>
-      </c>
-      <c r="AO1" s="25" t="s">
-        <v>505</v>
-      </c>
-      <c r="AP1" s="25" t="s">
-        <v>506</v>
-      </c>
-      <c r="AQ1" s="25" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="2" spans="1:51" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -4630,128 +4616,128 @@
         <v>81</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="45"/>
+      <c r="F2" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>505</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>506</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="L2" s="30" t="s">
         <v>508</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="M2" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>449</v>
+      </c>
+      <c r="O2" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="P2" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q2" s="28" t="s">
         <v>509</v>
       </c>
-      <c r="D2" s="46" t="s">
-        <v>422</v>
-      </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="G2" s="27" t="s">
+      <c r="R2" s="29" t="s">
         <v>510</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="S2" s="27" t="s">
         <v>511</v>
       </c>
-      <c r="I2" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="30" t="s">
+      <c r="T2" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="U2" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="W2" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="X2" s="28" t="s">
         <v>512</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="Y2" s="27" t="s">
         <v>513</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="Z2" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="AA2" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB2" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="AC2" s="27" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD2" s="27" t="s">
         <v>514</v>
       </c>
-      <c r="M2" s="30" t="s">
-        <v>514</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>455</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>429</v>
-      </c>
-      <c r="P2" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q2" s="28" t="s">
+      <c r="AE2" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF2" s="27" t="s">
         <v>515</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="AG2" s="27" t="s">
+        <v>321</v>
+      </c>
+      <c r="AH2" s="30" t="s">
         <v>516</v>
       </c>
-      <c r="S2" s="27" t="s">
-        <v>517</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="U2" s="29" t="s">
-        <v>429</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="W2" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>518</v>
-      </c>
-      <c r="Y2" s="27" t="s">
-        <v>519</v>
-      </c>
-      <c r="Z2" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="AA2" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="AB2" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="AC2" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="AD2" s="27" t="s">
-        <v>520</v>
-      </c>
-      <c r="AE2" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="AF2" s="27" t="s">
-        <v>521</v>
-      </c>
-      <c r="AG2" s="27" t="s">
-        <v>327</v>
-      </c>
-      <c r="AH2" s="30" t="s">
-        <v>522</v>
-      </c>
       <c r="AI2" s="30" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AJ2" s="27" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AK2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AL2" s="27" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="AM2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AN2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AO2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AP2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AQ2" s="27" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="AR2" s="28"/>
       <c r="AS2" s="28"/>
@@ -4814,82 +4800,82 @@
         <v>1</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E1" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>520</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>521</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>523</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>524</v>
       </c>
-      <c r="G1" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="H1" s="22" t="s">
+      <c r="N1" s="22" t="s">
         <v>525</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="O1" s="22" t="s">
         <v>526</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="P1" s="22" t="s">
         <v>527</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="Q1" s="22" t="s">
         <v>528</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="R1" s="22" t="s">
         <v>529</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="S1" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="T1" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="U1" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="V1" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="Q1" s="22" t="s">
+      <c r="W1" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="X1" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>539</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>540</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4897,83 +4883,83 @@
         <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>544</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>548</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>550</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>551</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>552</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>553</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="P2" s="35">
         <v>33.68</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="U2" s="36" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="W2" s="31" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="Z2" s="10" t="s">
         <v>81</v>
       </c>
       <c r="AA2" s="10"/>
       <c r="AB2" s="10" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature/GDE-9271 addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D595D078-686E-4112-BD74-134213E41FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125070D-77BB-4B6A-AFA8-85D69AB4578C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="822">
   <si>
     <t>rowid</t>
   </si>
@@ -2507,6 +2507,9 @@
   </si>
   <si>
     <t>140,000.00</t>
+  </si>
+  <si>
+    <t>Base_Rate</t>
   </si>
 </sst>
 </file>
@@ -3888,10 +3891,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3911,9 +3914,10 @@
     <col min="13" max="13" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="80" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
@@ -3959,8 +3963,11 @@
       <c r="O1" s="21" t="s">
         <v>648</v>
       </c>
+      <c r="P1" s="80" t="s">
+        <v>821</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" s="61" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="61" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
@@ -4006,8 +4013,11 @@
       <c r="O2" s="73" t="s">
         <v>663</v>
       </c>
+      <c r="P2" s="61" t="s">
+        <v>328</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="73"/>
       <c r="D5" s="73"/>
     </row>
@@ -4024,8 +4034,8 @@
   </sheetPr>
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feature/GDE-9270 addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6125DBDA-B2B0-4A6D-A76F-3843064FB16F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6A5A8-8106-4972-815A-00A320675F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="891">
   <si>
     <t>rowid</t>
   </si>
@@ -2971,7 +2971,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3251,6 +3251,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7484,8 +7487,8 @@
   </sheetPr>
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7710,7 +7713,9 @@
       <c r="L2" s="84" t="s">
         <v>679</v>
       </c>
-      <c r="M2" s="22"/>
+      <c r="M2" s="97" t="s">
+        <v>328</v>
+      </c>
       <c r="N2" s="84" t="s">
         <v>680</v>
       </c>
@@ -7815,7 +7820,9 @@
       <c r="L3" s="84" t="s">
         <v>692</v>
       </c>
-      <c r="M3" s="22"/>
+      <c r="M3" s="97" t="s">
+        <v>328</v>
+      </c>
       <c r="N3" s="84" t="s">
         <v>680</v>
       </c>

</xml_diff>

<commit_message>
feature/GDE-9273 Collect Interest for PIM Future BILAT
Added new high level keyword
Updated data set
Added new variables
Added new keywords and updated existing keywords to handle scenario
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6A5A8-8106-4972-815A-00A320675F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7079D984-173B-4598-9A7B-E10009F80FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1471" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="898">
   <si>
     <t>rowid</t>
   </si>
@@ -1996,6 +1996,9 @@
     <t>Loan_AccrualEndDate</t>
   </si>
   <si>
+    <t>Borrower_BaseRate</t>
+  </si>
+  <si>
     <t>AcceptRate_FromPricing</t>
   </si>
   <si>
@@ -2104,7 +2107,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>60002094</t>
+    <t>60002126</t>
   </si>
   <si>
     <t>323.82</t>
@@ -2563,6 +2566,9 @@
     <t>InterestCapitalization_Status</t>
   </si>
   <si>
+    <t>InterestCapitalization_Status2</t>
+  </si>
+  <si>
     <t>Paperclip_EffectiveDate</t>
   </si>
   <si>
@@ -2587,6 +2593,12 @@
     <t>Breakfunding_Reason</t>
   </si>
   <si>
+    <t>GLShortName</t>
+  </si>
+  <si>
+    <t>CashFlow_AfterStatus</t>
+  </si>
+  <si>
     <t>SBLC_CycleNumber</t>
   </si>
   <si>
@@ -2644,6 +2656,15 @@
     <t>Borrower Decision</t>
   </si>
   <si>
+    <t>Special Acc't Pay.</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update to </t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -2707,7 +2728,7 @@
     <t>33.3333</t>
   </si>
   <si>
-    <t>Borrower_BaseRate</t>
+    <t>12-Jun-2023</t>
   </si>
 </sst>
 </file>
@@ -2971,7 +2992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3216,9 +3237,6 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3253,8 +3271,14 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3936,16 +3960,16 @@
       <c r="A2" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>83</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>85</v>
       </c>
       <c r="F2" s="63" t="s">
@@ -3957,7 +3981,7 @@
       <c r="H2" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="89" t="s">
         <v>88</v>
       </c>
       <c r="J2" s="63" t="s">
@@ -4022,10 +4046,10 @@
       <c r="AG2" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="AH2" s="84" t="s">
+      <c r="AH2" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="AI2" s="84" t="s">
+      <c r="AI2" s="96" t="s">
         <v>90</v>
       </c>
       <c r="AJ2" s="36"/>
@@ -4076,29 +4100,29 @@
       <c r="CC2" s="24"/>
       <c r="CD2" s="24"/>
       <c r="CE2" s="24"/>
-      <c r="CF2" s="84"/>
-      <c r="CG2" s="84"/>
-      <c r="CH2" s="84"/>
-      <c r="CI2" s="84"/>
-      <c r="CJ2" s="84"/>
-      <c r="CK2" s="84"/>
-      <c r="CL2" s="84"/>
-      <c r="CM2" s="84"/>
-      <c r="CN2" s="84"/>
-      <c r="CO2" s="84"/>
-      <c r="CP2" s="84"/>
-      <c r="CQ2" s="84"/>
-      <c r="CR2" s="84"/>
-      <c r="CS2" s="84"/>
-      <c r="CT2" s="84"/>
-      <c r="CU2" s="84"/>
-      <c r="CV2" s="84"/>
-      <c r="CW2" s="84"/>
-      <c r="CX2" s="84"/>
-      <c r="CY2" s="84"/>
-      <c r="CZ2" s="84"/>
-      <c r="DA2" s="84"/>
-      <c r="DB2" s="84"/>
+      <c r="CF2" s="96"/>
+      <c r="CG2" s="96"/>
+      <c r="CH2" s="96"/>
+      <c r="CI2" s="96"/>
+      <c r="CJ2" s="96"/>
+      <c r="CK2" s="96"/>
+      <c r="CL2" s="96"/>
+      <c r="CM2" s="96"/>
+      <c r="CN2" s="96"/>
+      <c r="CO2" s="96"/>
+      <c r="CP2" s="96"/>
+      <c r="CQ2" s="96"/>
+      <c r="CR2" s="96"/>
+      <c r="CS2" s="96"/>
+      <c r="CT2" s="96"/>
+      <c r="CU2" s="96"/>
+      <c r="CV2" s="96"/>
+      <c r="CW2" s="96"/>
+      <c r="CX2" s="96"/>
+      <c r="CY2" s="96"/>
+      <c r="CZ2" s="96"/>
+      <c r="DA2" s="96"/>
+      <c r="DB2" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4148,7 +4172,7 @@
         <v>334</v>
       </c>
       <c r="D1" s="77" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E1" s="78" t="s">
         <v>336</v>
@@ -4157,89 +4181,89 @@
         <v>641</v>
       </c>
       <c r="G1" s="78" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H1" s="79" t="s">
         <v>642</v>
       </c>
       <c r="I1" s="80" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="J1" s="80" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="K1" s="77" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="L1" s="77" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="M1" s="77" t="s">
         <v>644</v>
       </c>
       <c r="N1" s="77" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="P1" s="77" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="60" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>421</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>285</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="84" t="s">
-        <v>675</v>
-      </c>
-      <c r="G2" s="84" t="s">
-        <v>798</v>
-      </c>
-      <c r="H2" s="84" t="s">
+      <c r="F2" s="96" t="s">
+        <v>676</v>
+      </c>
+      <c r="G2" s="96" t="s">
+        <v>799</v>
+      </c>
+      <c r="H2" s="96" t="s">
         <v>238</v>
       </c>
       <c r="I2" s="83">
         <v>3854477.59</v>
       </c>
-      <c r="J2" s="84">
+      <c r="J2" s="96">
         <v>100</v>
       </c>
       <c r="K2" s="82" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="L2" s="82" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="M2" s="82" t="s">
         <v>434</v>
       </c>
       <c r="N2" s="60" t="s">
-        <v>679</v>
-      </c>
-      <c r="O2" s="84" t="s">
-        <v>681</v>
+        <v>680</v>
+      </c>
+      <c r="O2" s="96" t="s">
+        <v>682</v>
       </c>
       <c r="P2" s="60" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4252,10 +4276,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W39" sqref="W39"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4263,7 +4287,7 @@
     <col min="1" max="1" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -4275,29 +4299,31 @@
     <col min="14" max="14" width="23.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22" style="2" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="40.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="26" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -4305,192 +4331,225 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>843</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>595</v>
       </c>
-      <c r="E1" s="26" t="s">
-        <v>842</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H1" s="26" t="s">
+        <v>846</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>645</v>
       </c>
-      <c r="I1" s="26" t="s">
-        <v>845</v>
-      </c>
       <c r="J1" s="26" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="M1" s="26" t="s">
+        <v>850</v>
+      </c>
+      <c r="N1" s="26" t="s">
         <v>644</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>592</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="P1" s="31" t="s">
-        <v>849</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>744</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>850</v>
-      </c>
-      <c r="S1" s="26" t="s">
+      <c r="Q1" s="31" t="s">
         <v>851</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="R1" s="31" t="s">
         <v>852</v>
       </c>
+      <c r="S1" s="31" t="s">
+        <v>853</v>
+      </c>
+      <c r="T1" s="31" t="s">
+        <v>605</v>
+      </c>
       <c r="U1" s="26" t="s">
-        <v>853</v>
+        <v>745</v>
       </c>
       <c r="V1" s="26" t="s">
-        <v>749</v>
+        <v>854</v>
       </c>
       <c r="W1" s="26" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="X1" s="26" t="s">
-        <v>855</v>
-      </c>
-      <c r="Y1" s="31" t="s">
+        <v>856</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>857</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>750</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>858</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>859</v>
+      </c>
+      <c r="AC1" s="31" t="s">
         <v>606</v>
       </c>
-      <c r="Z1" s="31" t="s">
+      <c r="AD1" s="31" t="s">
         <v>607</v>
       </c>
-      <c r="AA1" s="31" t="s">
+      <c r="AE1" s="31" t="s">
         <v>608</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>593</v>
       </c>
-      <c r="AC1" s="26" t="s">
-        <v>856</v>
-      </c>
-      <c r="AD1" s="26" t="s">
-        <v>837</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>857</v>
-      </c>
-      <c r="AF1" s="26" t="s">
-        <v>858</v>
-      </c>
       <c r="AG1" s="26" t="s">
-        <v>859</v>
-      </c>
-      <c r="AH1" s="31" t="s">
+        <v>860</v>
+      </c>
+      <c r="AH1" s="26" t="s">
+        <v>838</v>
+      </c>
+      <c r="AI1" s="26" t="s">
+        <v>861</v>
+      </c>
+      <c r="AJ1" s="26" t="s">
+        <v>862</v>
+      </c>
+      <c r="AK1" s="26" t="s">
+        <v>863</v>
+      </c>
+      <c r="AL1" s="31" t="s">
         <v>597</v>
       </c>
-      <c r="AI1" s="31" t="s">
+      <c r="AM1" s="31" t="s">
         <v>598</v>
       </c>
-      <c r="AJ1" s="31" t="s">
+      <c r="AN1" s="31" t="s">
         <v>599</v>
       </c>
-      <c r="AK1" s="31" t="s">
+      <c r="AO1" s="31" t="s">
         <v>600</v>
       </c>
-      <c r="AL1" s="31" t="s">
+      <c r="AP1" s="31" t="s">
         <v>601</v>
       </c>
-      <c r="AM1" s="31" t="s">
+      <c r="AQ1" s="31" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="30" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+    <row r="2" spans="1:43" s="30" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="85" t="s">
-        <v>860</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>691</v>
-      </c>
-      <c r="F2" s="85" t="s">
-        <v>861</v>
-      </c>
-      <c r="G2" s="85" t="s">
-        <v>862</v>
-      </c>
-      <c r="H2" s="86" t="s">
-        <v>863</v>
-      </c>
-      <c r="I2" s="86" t="s">
+      <c r="D2" s="96" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" s="84" t="s">
         <v>864</v>
       </c>
-      <c r="J2" s="86" t="s">
+      <c r="F2" s="84" t="s">
+        <v>692</v>
+      </c>
+      <c r="G2" s="84" t="s">
         <v>865</v>
       </c>
+      <c r="H2" s="84" t="s">
+        <v>866</v>
+      </c>
+      <c r="I2" s="85" t="s">
+        <v>867</v>
+      </c>
+      <c r="J2" s="85" t="s">
+        <v>868</v>
+      </c>
       <c r="K2" s="85" t="s">
+        <v>869</v>
+      </c>
+      <c r="L2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="85" t="s">
-        <v>866</v>
-      </c>
-      <c r="M2" s="85" t="s">
-        <v>867</v>
+      <c r="M2" s="84" t="s">
+        <v>870</v>
       </c>
       <c r="N2" s="84" t="s">
+        <v>871</v>
+      </c>
+      <c r="O2" s="96" t="s">
         <v>426</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="P2" s="96" t="s">
         <v>426</v>
       </c>
-      <c r="P2" s="84" t="s">
-        <v>868</v>
-      </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
+      <c r="Q2" s="96" t="s">
+        <v>872</v>
+      </c>
+      <c r="R2" s="96" t="s">
+        <v>873</v>
+      </c>
+      <c r="S2" s="96" t="s">
+        <v>874</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>897</v>
+      </c>
+      <c r="U2" s="44"/>
       <c r="V2" s="33"/>
       <c r="W2" s="33"/>
       <c r="X2" s="33"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="35"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
       <c r="AF2" s="24"/>
       <c r="AG2" s="33"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="35"/>
       <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="24"/>
+      <c r="AO2" s="24"/>
+      <c r="AP2" s="24"/>
+      <c r="AQ2" s="24"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="S4" s="97" t="s">
+        <v>875</v>
+      </c>
+      <c r="T4" s="98" t="s">
+        <v>692</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4501,8 +4560,8 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4543,7 +4602,7 @@
     <col min="34" max="37" width="15" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="89" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="88" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -4551,13 +4610,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>334</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>336</v>
@@ -4566,31 +4625,31 @@
         <v>641</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>872</v>
-      </c>
-      <c r="L1" s="91" t="s">
+        <v>879</v>
+      </c>
+      <c r="L1" s="90" t="s">
         <v>107</v>
       </c>
       <c r="M1" s="31" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="N1" s="31" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="O1" s="31" t="s">
-        <v>875</v>
+        <v>882</v>
       </c>
       <c r="P1" s="31" t="s">
-        <v>876</v>
+        <v>883</v>
       </c>
       <c r="Q1" s="26" t="s">
         <v>606</v>
@@ -4611,89 +4670,89 @@
         <v>602</v>
       </c>
       <c r="W1" s="26" t="s">
-        <v>877</v>
-      </c>
-      <c r="X1" s="87" t="s">
+        <v>884</v>
+      </c>
+      <c r="X1" s="86" t="s">
         <v>593</v>
       </c>
       <c r="Y1" s="31" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="Z1" s="31" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="AA1" s="31" t="s">
-        <v>726</v>
-      </c>
-      <c r="AB1" s="88" t="s">
+        <v>727</v>
+      </c>
+      <c r="AB1" s="87" t="s">
         <v>338</v>
       </c>
-      <c r="AC1" s="88" t="s">
-        <v>878</v>
-      </c>
-      <c r="AD1" s="88" t="s">
+      <c r="AC1" s="87" t="s">
+        <v>885</v>
+      </c>
+      <c r="AD1" s="87" t="s">
         <v>592</v>
       </c>
-      <c r="AE1" s="88" t="s">
+      <c r="AE1" s="87" t="s">
         <v>167</v>
       </c>
       <c r="AF1" s="31" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="AG1" s="31" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="AH1" s="31" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="AI1" s="31" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="89" t="s">
         <v>285</v>
       </c>
       <c r="D2" s="24"/>
-      <c r="E2" s="90" t="s">
-        <v>879</v>
+      <c r="E2" s="89" t="s">
+        <v>886</v>
       </c>
       <c r="F2" s="24"/>
-      <c r="G2" t="s">
-        <v>798</v>
-      </c>
-      <c r="H2" s="90" t="s">
+      <c r="G2" s="94" t="s">
+        <v>799</v>
+      </c>
+      <c r="H2" s="89" t="s">
         <v>574</v>
       </c>
-      <c r="I2" s="90" t="s">
+      <c r="I2" s="89" t="s">
         <v>270</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>427</v>
       </c>
-      <c r="K2" s="85" t="s">
-        <v>880</v>
-      </c>
-      <c r="L2" s="85" t="s">
-        <v>881</v>
-      </c>
-      <c r="M2" s="85" t="s">
-        <v>882</v>
-      </c>
-      <c r="N2" s="85" t="s">
-        <v>883</v>
-      </c>
-      <c r="O2" s="85" t="s">
-        <v>884</v>
-      </c>
-      <c r="P2" s="92" t="s">
-        <v>885</v>
+      <c r="K2" s="84" t="s">
+        <v>887</v>
+      </c>
+      <c r="L2" s="84" t="s">
+        <v>888</v>
+      </c>
+      <c r="M2" s="84" t="s">
+        <v>889</v>
+      </c>
+      <c r="N2" s="84" t="s">
+        <v>890</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>891</v>
+      </c>
+      <c r="P2" s="91" t="s">
+        <v>892</v>
       </c>
       <c r="Q2" s="35" t="s">
         <v>308</v>
@@ -4715,16 +4774,16 @@
       </c>
       <c r="W2" s="35"/>
       <c r="X2" s="33" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
       <c r="Y2" s="35" t="s">
         <v>270</v>
       </c>
       <c r="Z2" s="35" t="s">
-        <v>887</v>
+        <v>894</v>
       </c>
       <c r="AA2" s="35" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="AB2" s="24" t="s">
         <v>513</v>
@@ -4739,16 +4798,16 @@
         <v>451</v>
       </c>
       <c r="AF2" s="33" t="s">
-        <v>888</v>
+        <v>895</v>
       </c>
       <c r="AG2" s="24" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
       <c r="AH2" s="24" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
       <c r="AI2" s="24" t="s">
-        <v>889</v>
+        <v>896</v>
       </c>
     </row>
   </sheetData>
@@ -4764,8 +4823,8 @@
   </sheetPr>
   <dimension ref="A1:EE2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView topLeftCell="DK1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DQ2" sqref="DQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5313,10 +5372,10 @@
       </c>
     </row>
     <row r="2" spans="1:135" s="60" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
       <c r="C2" s="48" t="s">
@@ -5364,7 +5423,7 @@
       <c r="Q2" s="49" t="s">
         <v>249</v>
       </c>
-      <c r="R2" s="84" t="s">
+      <c r="R2" s="96" t="s">
         <v>250</v>
       </c>
       <c r="S2" s="50" t="s">
@@ -5448,29 +5507,29 @@
       <c r="AS2" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="AT2" s="90"/>
-      <c r="AU2" s="90" t="s">
+      <c r="AT2" s="89"/>
+      <c r="AU2" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="AV2" s="90" t="s">
+      <c r="AV2" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="AW2" s="90" t="s">
+      <c r="AW2" s="89" t="s">
         <v>90</v>
       </c>
       <c r="AX2" s="54" t="s">
         <v>273</v>
       </c>
-      <c r="AY2" s="90" t="s">
+      <c r="AY2" s="89" t="s">
         <v>274</v>
       </c>
       <c r="AZ2" s="49" t="s">
         <v>275</v>
       </c>
-      <c r="BA2" s="90" t="s">
+      <c r="BA2" s="89" t="s">
         <v>276</v>
       </c>
-      <c r="BB2" s="90" t="s">
+      <c r="BB2" s="89" t="s">
         <v>277</v>
       </c>
       <c r="BC2" s="55" t="s">
@@ -5479,22 +5538,22 @@
       <c r="BD2" s="55" t="s">
         <v>279</v>
       </c>
-      <c r="BE2" s="90" t="s">
+      <c r="BE2" s="89" t="s">
         <v>280</v>
       </c>
-      <c r="BF2" s="90" t="s">
+      <c r="BF2" s="89" t="s">
         <v>281</v>
       </c>
-      <c r="BG2" s="90" t="s">
+      <c r="BG2" s="89" t="s">
         <v>282</v>
       </c>
-      <c r="BH2" s="90" t="s">
+      <c r="BH2" s="89" t="s">
         <v>280</v>
       </c>
-      <c r="BI2" s="90" t="s">
+      <c r="BI2" s="89" t="s">
         <v>283</v>
       </c>
-      <c r="BJ2" s="90" t="s">
+      <c r="BJ2" s="89" t="s">
         <v>284</v>
       </c>
       <c r="BK2" s="49" t="s">
@@ -5503,10 +5562,10 @@
       <c r="BL2" s="49" t="s">
         <v>251</v>
       </c>
-      <c r="BM2" s="90" t="s">
+      <c r="BM2" s="89" t="s">
         <v>285</v>
       </c>
-      <c r="BN2" s="90" t="s">
+      <c r="BN2" s="89" t="s">
         <v>286</v>
       </c>
       <c r="BO2" s="35" t="s">
@@ -5729,8 +5788,8 @@
   </sheetPr>
   <dimension ref="A1:CL7"/>
   <sheetViews>
-    <sheetView topLeftCell="BL1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BR2" sqref="BR2"/>
+    <sheetView topLeftCell="AJ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6099,49 +6158,49 @@
       </c>
     </row>
     <row r="2" spans="1:90" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>419</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="96" t="s">
         <v>420</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="96" t="s">
         <v>422</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="96" t="s">
         <v>270</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="96" t="s">
         <v>245</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="96" t="s">
         <v>329</v>
       </c>
-      <c r="L2" s="84" t="s">
+      <c r="L2" s="96" t="s">
         <v>250</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="84" t="s">
         <v>424</v>
       </c>
-      <c r="N2" s="85" t="s">
+      <c r="N2" s="84" t="s">
         <v>425</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="96" t="s">
         <v>426</v>
       </c>
       <c r="P2" s="42" t="s">
@@ -6162,10 +6221,10 @@
       <c r="U2" s="42" t="s">
         <v>426</v>
       </c>
-      <c r="V2" s="84" t="s">
+      <c r="V2" s="96" t="s">
         <v>430</v>
       </c>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="96" t="s">
         <v>431</v>
       </c>
       <c r="X2" s="37" t="s">
@@ -6174,72 +6233,72 @@
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
       <c r="AA2" s="43"/>
-      <c r="AB2" s="84" t="s">
+      <c r="AB2" s="96" t="s">
         <v>241</v>
       </c>
-      <c r="AC2" s="84" t="s">
+      <c r="AC2" s="96" t="s">
         <v>277</v>
       </c>
-      <c r="AD2" s="84" t="s">
+      <c r="AD2" s="96" t="s">
         <v>240</v>
       </c>
-      <c r="AE2" s="84" t="s">
+      <c r="AE2" s="96" t="s">
         <v>433</v>
       </c>
-      <c r="AF2" s="84" t="s">
+      <c r="AF2" s="96" t="s">
         <v>434</v>
       </c>
-      <c r="AG2" s="84" t="s">
+      <c r="AG2" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="AH2" s="84" t="s">
+      <c r="AH2" s="96" t="s">
         <v>435</v>
       </c>
-      <c r="AI2" s="85" t="s">
+      <c r="AI2" s="84" t="s">
         <v>436</v>
       </c>
-      <c r="AJ2" s="85" t="s">
+      <c r="AJ2" s="84" t="s">
         <v>437</v>
       </c>
-      <c r="AK2" s="85" t="s">
+      <c r="AK2" s="84" t="s">
         <v>438</v>
       </c>
-      <c r="AL2" s="85" t="s">
+      <c r="AL2" s="84" t="s">
         <v>438</v>
       </c>
-      <c r="AM2" s="85" t="s">
+      <c r="AM2" s="84" t="s">
         <v>439</v>
       </c>
-      <c r="AN2" s="85" t="s">
+      <c r="AN2" s="84" t="s">
         <v>440</v>
       </c>
-      <c r="AO2" s="85" t="s">
+      <c r="AO2" s="84" t="s">
         <v>441</v>
       </c>
-      <c r="AP2" s="85" t="s">
+      <c r="AP2" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="AQ2" s="85" t="s">
+      <c r="AQ2" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="AR2" s="85" t="s">
+      <c r="AR2" s="84" t="s">
         <v>442</v>
       </c>
-      <c r="AS2" s="85" t="s">
+      <c r="AS2" s="84" t="s">
         <v>443</v>
       </c>
-      <c r="AT2" s="85" t="s">
+      <c r="AT2" s="84" t="s">
         <v>444</v>
       </c>
       <c r="AU2" s="33"/>
       <c r="AV2" s="33"/>
-      <c r="AW2" s="85" t="s">
+      <c r="AW2" s="84" t="s">
         <v>445</v>
       </c>
-      <c r="AX2" s="85" t="s">
+      <c r="AX2" s="84" t="s">
         <v>440</v>
       </c>
-      <c r="AY2" s="85" t="s">
+      <c r="AY2" s="84" t="s">
         <v>438</v>
       </c>
       <c r="AZ2" s="24" t="s">
@@ -6372,8 +6431,8 @@
   </sheetPr>
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:Z2"/>
+    <sheetView topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6544,28 +6603,28 @@
       </c>
     </row>
     <row r="2" spans="1:50" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="84" t="s">
         <v>505</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="84" t="s">
         <v>506</v>
       </c>
-      <c r="G2" s="90" t="s">
+      <c r="G2" s="89" t="s">
         <v>507</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="84" t="s">
         <v>270</v>
       </c>
       <c r="I2" s="37" t="s">
@@ -6580,40 +6639,40 @@
       <c r="L2" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="M2" s="84" t="s">
+      <c r="M2" s="96" t="s">
         <v>428</v>
       </c>
       <c r="N2" s="37" t="s">
         <v>427</v>
       </c>
-      <c r="O2" s="90" t="s">
+      <c r="O2" s="89" t="s">
         <v>285</v>
       </c>
-      <c r="P2" s="90" t="s">
+      <c r="P2" s="89" t="s">
         <v>509</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>510</v>
       </c>
-      <c r="R2" s="85" t="s">
+      <c r="R2" s="84" t="s">
         <v>509</v>
       </c>
-      <c r="S2" s="85" t="s">
+      <c r="S2" s="84" t="s">
         <v>511</v>
       </c>
-      <c r="T2" s="85" t="s">
+      <c r="T2" s="84" t="s">
         <v>282</v>
       </c>
-      <c r="U2" s="84" t="s">
+      <c r="U2" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="V2" s="85" t="s">
+      <c r="V2" s="84" t="s">
         <v>249</v>
       </c>
-      <c r="W2" s="85" t="s">
+      <c r="W2" s="84" t="s">
         <v>512</v>
       </c>
-      <c r="X2" s="85" t="s">
+      <c r="X2" s="84" t="s">
         <v>509</v>
       </c>
       <c r="Y2" s="38" t="s">
@@ -6878,103 +6937,103 @@
       <c r="A2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="96" t="s">
         <v>555</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>556</v>
       </c>
-      <c r="F2" s="84" t="s">
+      <c r="F2" s="96" t="s">
         <v>445</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="96" t="s">
         <v>463</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="96" t="s">
         <v>557</v>
       </c>
-      <c r="I2" s="84" t="s">
+      <c r="I2" s="96" t="s">
         <v>558</v>
       </c>
-      <c r="J2" s="84" t="s">
+      <c r="J2" s="96" t="s">
         <v>559</v>
       </c>
-      <c r="K2" s="84" t="s">
+      <c r="K2" s="96" t="s">
         <v>560</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="84" t="s">
         <v>561</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="84" t="s">
         <v>562</v>
       </c>
-      <c r="N2" s="85" t="s">
+      <c r="N2" s="84" t="s">
         <v>329</v>
       </c>
-      <c r="O2" s="85" t="s">
+      <c r="O2" s="84" t="s">
         <v>563</v>
       </c>
-      <c r="P2" s="85" t="s">
+      <c r="P2" s="84" t="s">
         <v>564</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>565</v>
       </c>
-      <c r="R2" s="85" t="s">
+      <c r="R2" s="84" t="s">
         <v>566</v>
       </c>
-      <c r="S2" s="85" t="s">
+      <c r="S2" s="84" t="s">
         <v>567</v>
       </c>
-      <c r="T2" s="85" t="s">
+      <c r="T2" s="84" t="s">
         <v>568</v>
       </c>
-      <c r="U2" s="90" t="s">
+      <c r="U2" s="89" t="s">
         <v>569</v>
       </c>
-      <c r="V2" s="85" t="s">
+      <c r="V2" s="84" t="s">
         <v>570</v>
       </c>
-      <c r="W2" s="85" t="s">
+      <c r="W2" s="84" t="s">
         <v>571</v>
       </c>
-      <c r="X2" s="85" t="s">
+      <c r="X2" s="84" t="s">
         <v>572</v>
       </c>
-      <c r="Y2" s="85" t="s">
+      <c r="Y2" s="84" t="s">
         <v>257</v>
       </c>
-      <c r="Z2" s="85">
+      <c r="Z2" s="84">
         <v>50</v>
       </c>
       <c r="AA2" s="9" t="s">
         <v>573</v>
       </c>
-      <c r="AB2" s="90" t="s">
+      <c r="AB2" s="89" t="s">
         <v>434</v>
       </c>
-      <c r="AC2" s="90" t="s">
+      <c r="AC2" s="89" t="s">
         <v>463</v>
       </c>
-      <c r="AD2" s="90">
+      <c r="AD2" s="89">
         <v>1.65</v>
       </c>
-      <c r="AE2" s="90" t="s">
+      <c r="AE2" s="89" t="s">
         <v>569</v>
       </c>
-      <c r="AF2" s="90" t="s">
+      <c r="AF2" s="89" t="s">
         <v>574</v>
       </c>
-      <c r="AG2" s="90" t="s">
+      <c r="AG2" s="89" t="s">
         <v>575</v>
       </c>
-      <c r="AH2" s="90" t="s">
+      <c r="AH2" s="89" t="s">
         <v>576</v>
       </c>
       <c r="AI2" s="35" t="s">
@@ -7011,8 +7070,8 @@
   </sheetPr>
   <dimension ref="A1:AK3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:AK1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7167,35 +7226,35 @@
         <v>609</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="85" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+    <row r="2" spans="1:37" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="84" t="s">
         <v>445</v>
       </c>
-      <c r="E2" s="84" t="s">
+      <c r="E2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="84" t="s">
         <v>610</v>
       </c>
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="84" t="s">
         <v>611</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="84" t="s">
         <v>612</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="I2" s="84" t="s">
         <v>613</v>
       </c>
-      <c r="J2" s="85" t="s">
+      <c r="J2" s="84" t="s">
         <v>614</v>
       </c>
       <c r="K2" s="65">
@@ -7210,19 +7269,19 @@
       <c r="N2" s="72">
         <v>875.27</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="P2" s="84" t="s">
+      <c r="P2" s="96" t="s">
         <v>426</v>
       </c>
-      <c r="Q2" s="85" t="s">
+      <c r="Q2" s="84" t="s">
         <v>426</v>
       </c>
-      <c r="R2" s="84" t="s">
+      <c r="R2" s="96" t="s">
         <v>615</v>
       </c>
-      <c r="S2" s="85" t="s">
+      <c r="S2" s="84" t="s">
         <v>81</v>
       </c>
       <c r="T2" s="33" t="s">
@@ -7400,16 +7459,16 @@
       <c r="AB1" s="19"/>
     </row>
     <row r="2" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="96" t="s">
         <v>423</v>
       </c>
       <c r="E2" s="28" t="s">
@@ -7442,32 +7501,32 @@
       <c r="N2" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="O2" s="84" t="s">
+      <c r="O2" s="96" t="s">
         <v>454</v>
       </c>
-      <c r="P2" s="84" t="s">
+      <c r="P2" s="96" t="s">
         <v>452</v>
       </c>
-      <c r="Q2" s="84" t="s">
+      <c r="Q2" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="85" t="s">
+      <c r="R2" s="84" t="s">
         <v>432</v>
       </c>
-      <c r="S2" s="85" t="s">
+      <c r="S2" s="84" t="s">
         <v>432</v>
       </c>
-      <c r="T2" s="84" t="s">
+      <c r="T2" s="96" t="s">
         <v>639</v>
       </c>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="N3" s="3" t="s">
@@ -7487,8 +7546,8 @@
   </sheetPr>
   <dimension ref="A1:AS8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7595,52 +7654,52 @@
         <v>592</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>890</v>
+        <v>653</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="AF1" s="21" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="AG1" s="20" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="AH1" s="20" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="AI1" s="20" t="s">
         <v>599</v>
@@ -7655,119 +7714,119 @@
         <v>602</v>
       </c>
       <c r="AM1" s="20" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="AN1" s="20" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="AO1" s="20" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="AP1" s="19" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="AQ1" s="19" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="AR1" s="19" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="AS1" s="19" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="E2" s="84" t="s">
-        <v>675</v>
-      </c>
-      <c r="F2" s="84" t="s">
+      <c r="E2" s="96" t="s">
+        <v>676</v>
+      </c>
+      <c r="F2" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="96" t="s">
         <v>285</v>
       </c>
-      <c r="H2" s="84" t="s">
+      <c r="H2" s="96" t="s">
         <v>434</v>
       </c>
-      <c r="I2" s="90" t="s">
-        <v>676</v>
-      </c>
-      <c r="J2" s="85" t="s">
+      <c r="I2" s="89" t="s">
         <v>677</v>
       </c>
+      <c r="J2" s="84" t="s">
+        <v>678</v>
+      </c>
       <c r="K2" s="14" t="s">
-        <v>678</v>
-      </c>
-      <c r="L2" s="84" t="s">
         <v>679</v>
       </c>
-      <c r="M2" s="97" t="s">
+      <c r="L2" s="96" t="s">
+        <v>680</v>
+      </c>
+      <c r="M2" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="N2" s="84" t="s">
-        <v>680</v>
-      </c>
-      <c r="O2" s="85" t="s">
+      <c r="N2" s="96" t="s">
+        <v>681</v>
+      </c>
+      <c r="O2" s="84" t="s">
         <v>614</v>
       </c>
-      <c r="P2" s="85" t="s">
+      <c r="P2" s="84" t="s">
         <v>614</v>
       </c>
-      <c r="Q2" s="84" t="s">
+      <c r="Q2" s="96" t="s">
         <v>426</v>
       </c>
-      <c r="R2" s="84" t="s">
+      <c r="R2" s="96" t="s">
         <v>426</v>
       </c>
-      <c r="S2" s="84" t="s">
+      <c r="S2" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="T2" s="84" t="s">
-        <v>681</v>
-      </c>
-      <c r="U2" s="84" t="s">
+      <c r="T2" s="96" t="s">
         <v>682</v>
+      </c>
+      <c r="U2" s="96" t="s">
+        <v>683</v>
       </c>
       <c r="V2" s="23"/>
       <c r="W2" s="23"/>
-      <c r="X2" s="90" t="s">
-        <v>676</v>
-      </c>
-      <c r="Y2" s="90" t="s">
-        <v>676</v>
-      </c>
-      <c r="Z2" s="90" t="s">
-        <v>676</v>
-      </c>
-      <c r="AA2" s="90" t="s">
-        <v>676</v>
-      </c>
-      <c r="AB2" s="94" t="s">
-        <v>683</v>
-      </c>
-      <c r="AC2" s="94" t="s">
+      <c r="X2" s="89" t="s">
+        <v>677</v>
+      </c>
+      <c r="Y2" s="89" t="s">
+        <v>677</v>
+      </c>
+      <c r="Z2" s="89" t="s">
+        <v>677</v>
+      </c>
+      <c r="AA2" s="89" t="s">
+        <v>677</v>
+      </c>
+      <c r="AB2" s="93" t="s">
         <v>684</v>
       </c>
-      <c r="AD2" s="96" t="s">
+      <c r="AC2" s="93" t="s">
         <v>685</v>
       </c>
-      <c r="AE2" s="96" t="s">
+      <c r="AD2" s="95" t="s">
         <v>686</v>
       </c>
-      <c r="AF2" s="96" t="s">
+      <c r="AE2" s="95" t="s">
         <v>687</v>
+      </c>
+      <c r="AF2" s="95" t="s">
+        <v>688</v>
       </c>
       <c r="AG2" s="23"/>
       <c r="AH2" s="23"/>
@@ -7784,101 +7843,101 @@
       <c r="AS2" s="24"/>
     </row>
     <row r="3" spans="1:45" s="25" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
-        <v>688</v>
-      </c>
-      <c r="B3" s="84" t="s">
+      <c r="A3" s="96" t="s">
+        <v>689</v>
+      </c>
+      <c r="B3" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="96" t="s">
         <v>421</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="96" t="s">
         <v>423</v>
       </c>
-      <c r="E3" s="84" t="s">
-        <v>689</v>
-      </c>
-      <c r="F3" s="84" t="s">
+      <c r="E3" s="96" t="s">
+        <v>690</v>
+      </c>
+      <c r="F3" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="G3" s="84" t="s">
+      <c r="G3" s="96" t="s">
         <v>285</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="96" t="s">
         <v>434</v>
       </c>
-      <c r="I3" s="90" t="s">
-        <v>690</v>
-      </c>
-      <c r="J3" s="85" t="s">
+      <c r="I3" s="89" t="s">
         <v>691</v>
       </c>
+      <c r="J3" s="84" t="s">
+        <v>692</v>
+      </c>
       <c r="K3" s="14" t="s">
-        <v>678</v>
-      </c>
-      <c r="L3" s="84" t="s">
-        <v>692</v>
-      </c>
-      <c r="M3" s="97" t="s">
+        <v>679</v>
+      </c>
+      <c r="L3" s="96" t="s">
+        <v>693</v>
+      </c>
+      <c r="M3" s="96" t="s">
         <v>328</v>
       </c>
-      <c r="N3" s="84" t="s">
-        <v>680</v>
-      </c>
-      <c r="O3" s="85" t="s">
+      <c r="N3" s="96" t="s">
+        <v>681</v>
+      </c>
+      <c r="O3" s="84" t="s">
+        <v>694</v>
+      </c>
+      <c r="P3" s="84" t="s">
+        <v>694</v>
+      </c>
+      <c r="Q3" s="96" t="s">
+        <v>426</v>
+      </c>
+      <c r="R3" s="96" t="s">
+        <v>426</v>
+      </c>
+      <c r="S3" s="96" t="s">
+        <v>328</v>
+      </c>
+      <c r="T3" s="96" t="s">
+        <v>682</v>
+      </c>
+      <c r="U3" s="96" t="s">
+        <v>683</v>
+      </c>
+      <c r="V3" s="96" t="s">
+        <v>695</v>
+      </c>
+      <c r="W3" s="96" t="s">
+        <v>696</v>
+      </c>
+      <c r="X3" s="89" t="s">
+        <v>691</v>
+      </c>
+      <c r="Y3" s="89" t="s">
+        <v>691</v>
+      </c>
+      <c r="Z3" s="89" t="s">
+        <v>691</v>
+      </c>
+      <c r="AA3" s="89" t="s">
+        <v>691</v>
+      </c>
+      <c r="AB3" s="93" t="s">
+        <v>684</v>
+      </c>
+      <c r="AC3" s="96" t="s">
         <v>693</v>
       </c>
-      <c r="P3" s="85" t="s">
-        <v>693</v>
-      </c>
-      <c r="Q3" s="84" t="s">
-        <v>426</v>
-      </c>
-      <c r="R3" s="84" t="s">
-        <v>426</v>
-      </c>
-      <c r="S3" s="84" t="s">
-        <v>328</v>
-      </c>
-      <c r="T3" s="84" t="s">
-        <v>681</v>
-      </c>
-      <c r="U3" s="84" t="s">
-        <v>682</v>
-      </c>
-      <c r="V3" s="84" t="s">
-        <v>694</v>
-      </c>
-      <c r="W3" s="84" t="s">
-        <v>695</v>
-      </c>
-      <c r="X3" s="90" t="s">
-        <v>690</v>
-      </c>
-      <c r="Y3" s="90" t="s">
-        <v>690</v>
-      </c>
-      <c r="Z3" s="90" t="s">
-        <v>690</v>
-      </c>
-      <c r="AA3" s="90" t="s">
-        <v>690</v>
-      </c>
-      <c r="AB3" s="94" t="s">
-        <v>683</v>
-      </c>
-      <c r="AC3" s="84" t="s">
-        <v>692</v>
-      </c>
-      <c r="AD3" s="85" t="s">
-        <v>696</v>
-      </c>
-      <c r="AE3" s="96" t="s">
-        <v>686</v>
-      </c>
-      <c r="AF3" s="85" t="s">
+      <c r="AD3" s="84" t="s">
         <v>697</v>
+      </c>
+      <c r="AE3" s="95" t="s">
+        <v>687</v>
+      </c>
+      <c r="AF3" s="84" t="s">
+        <v>698</v>
       </c>
       <c r="AG3" s="23"/>
       <c r="AH3" s="23"/>
@@ -7912,8 +7971,8 @@
   </sheetPr>
   <dimension ref="A1:BL10"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ15" sqref="AJ15"/>
+    <sheetView topLeftCell="AK1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AW10" sqref="AW10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7999,100 +8058,100 @@
         <v>641</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="AB1" s="4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="AC1" s="7" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="AD1" s="7" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="AE1" s="7" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="AF1" s="68" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="AG1" s="7" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="AH1" s="4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="AJ1" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="AK1" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="AL1" s="8" t="s">
         <v>582</v>
@@ -8104,19 +8163,19 @@
         <v>590</v>
       </c>
       <c r="AO1" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="AP1" s="5" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="AQ1" s="5" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="AR1" s="5" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="AS1" s="5" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="AT1" s="5" t="s">
         <v>646</v>
@@ -8125,55 +8184,55 @@
         <v>647</v>
       </c>
       <c r="AV1" s="5" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="AW1" s="5" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="AX1" s="5" t="s">
         <v>651</v>
       </c>
       <c r="AY1" s="5" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="BA1" s="5" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="BB1" s="5" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="BC1" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="BD1" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="BE1" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="BF1" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="BG1" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="BH1" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="BI1" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="BJ1" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="BK1" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="BL1" s="5" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="2" spans="1:64" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8181,7 +8240,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>421</v>
@@ -8190,90 +8249,90 @@
         <v>423</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F2" s="9">
         <v>1100</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>238</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC2" s="9"/>
       <c r="AD2" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE2" s="10"/>
       <c r="AF2" s="69"/>
       <c r="AG2" s="9"/>
       <c r="AH2" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI2" s="9"/>
       <c r="AJ2" s="9" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="AK2" s="9"/>
       <c r="AL2" s="9"/>
@@ -8284,16 +8343,16 @@
       <c r="AQ2" s="9"/>
       <c r="AR2" s="9"/>
       <c r="AS2" s="9"/>
-      <c r="AT2" s="85" t="s">
-        <v>677</v>
+      <c r="AT2" s="84" t="s">
+        <v>678</v>
       </c>
       <c r="AU2" s="14" t="s">
         <v>508</v>
       </c>
       <c r="AV2" s="9" t="s">
-        <v>774</v>
-      </c>
-      <c r="AW2" s="85" t="s">
+        <v>775</v>
+      </c>
+      <c r="AW2" s="84" t="s">
         <v>614</v>
       </c>
       <c r="AX2" s="9"/>
@@ -8316,10 +8375,10 @@
     </row>
     <row r="3" spans="1:64" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>421</v>
@@ -8328,90 +8387,90 @@
         <v>423</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F3" s="9">
         <v>1100</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>238</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA3" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC3" s="9"/>
       <c r="AD3" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE3" s="10"/>
       <c r="AF3" s="69"/>
       <c r="AG3" s="9"/>
       <c r="AH3" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI3" s="9"/>
       <c r="AJ3" s="9" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="AK3" s="9"/>
       <c r="AL3" s="15"/>
@@ -8428,16 +8487,16 @@
         <v>2.6450000000000001E-2</v>
       </c>
       <c r="AS3" s="70" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AT3" s="16" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AU3" s="17" t="s">
         <v>508</v>
       </c>
       <c r="AV3" s="15" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="AW3" s="16" t="s">
         <v>614</v>
@@ -8465,7 +8524,7 @@
         <v>443</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>421</v>
@@ -8474,90 +8533,90 @@
         <v>423</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="F4" s="9">
         <v>1100</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="H4" s="18" t="s">
         <v>238</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q4" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="X4" s="10" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="Z4" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="AC4" s="10"/>
       <c r="AD4" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE4" s="10"/>
       <c r="AF4" s="69"/>
       <c r="AG4" s="9"/>
       <c r="AH4" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI4" s="9"/>
       <c r="AJ4" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="AK4" s="9"/>
       <c r="AL4" s="9" t="s">
@@ -8604,10 +8663,10 @@
     </row>
     <row r="5" spans="1:64" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>421</v>
@@ -8615,91 +8674,91 @@
       <c r="D5" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E5" s="84" t="s">
-        <v>798</v>
+      <c r="E5" s="96" t="s">
+        <v>799</v>
       </c>
       <c r="F5" s="9">
         <v>1100</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>238</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q5" s="9" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="Y5" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="Z5" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA5" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC5" s="9"/>
       <c r="AD5" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE5" s="10"/>
       <c r="AF5" s="69"/>
       <c r="AG5" s="9"/>
       <c r="AH5" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI5" s="9"/>
       <c r="AJ5" s="9" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="AK5" s="9"/>
       <c r="AL5" s="15"/>
@@ -8716,16 +8775,16 @@
         <v>2.6450000000000001E-2</v>
       </c>
       <c r="AS5" s="70" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="AT5" s="16" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AU5" s="17" t="s">
         <v>508</v>
       </c>
       <c r="AV5" s="15" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="AW5" s="16" t="s">
         <v>614</v>
@@ -8753,7 +8812,7 @@
         <v>580</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>421</v>
@@ -8761,91 +8820,91 @@
       <c r="D6" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E6" s="84" t="s">
-        <v>798</v>
+      <c r="E6" s="96" t="s">
+        <v>799</v>
       </c>
       <c r="F6" s="9">
         <v>1100</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>238</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q6" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC6" s="9"/>
       <c r="AD6" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="69"/>
       <c r="AG6" s="9"/>
       <c r="AH6" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI6" s="9"/>
       <c r="AJ6" s="9" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
@@ -8856,16 +8915,16 @@
       <c r="AQ6" s="9"/>
       <c r="AR6" s="9"/>
       <c r="AS6" s="9"/>
-      <c r="AT6" s="85" t="s">
-        <v>677</v>
+      <c r="AT6" s="84" t="s">
+        <v>678</v>
       </c>
       <c r="AU6" s="14" t="s">
         <v>508</v>
       </c>
       <c r="AV6" s="9" t="s">
-        <v>774</v>
-      </c>
-      <c r="AW6" s="85" t="s">
+        <v>775</v>
+      </c>
+      <c r="AW6" s="84" t="s">
         <v>614</v>
       </c>
       <c r="AX6" s="9"/>
@@ -8888,10 +8947,10 @@
     </row>
     <row r="7" spans="1:64" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>421</v>
@@ -8899,91 +8958,91 @@
       <c r="D7" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E7" s="84" t="s">
-        <v>798</v>
+      <c r="E7" s="96" t="s">
+        <v>799</v>
       </c>
       <c r="F7" s="9">
         <v>1100</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>238</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T7" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="W7" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="X7" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="Z7" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA7" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC7" s="10"/>
       <c r="AD7" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="69"/>
       <c r="AG7" s="9"/>
       <c r="AH7" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI7" s="9"/>
       <c r="AJ7" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="AK7" s="9"/>
       <c r="AL7" s="9" t="s">
@@ -9026,10 +9085,10 @@
     </row>
     <row r="8" spans="1:64" s="73" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>421</v>
@@ -9037,125 +9096,125 @@
       <c r="D8" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E8" s="84" t="s">
-        <v>798</v>
+      <c r="E8" s="96" t="s">
+        <v>799</v>
       </c>
       <c r="F8" s="9">
         <v>1100</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>236</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q8" s="9" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U8" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="Y8" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="Z8" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA8" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB8" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC8" s="10"/>
       <c r="AD8" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="69"/>
       <c r="AG8" s="9"/>
       <c r="AH8" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI8" s="9"/>
       <c r="AJ8" s="9" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="AK8" s="9"/>
       <c r="AL8" s="9"/>
       <c r="AM8" s="75"/>
       <c r="AN8" s="18"/>
-      <c r="AO8" s="93">
+      <c r="AO8" s="92">
         <v>12</v>
       </c>
       <c r="AP8" s="11" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="AQ8" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="AR8" s="76" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="AS8" s="11" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="AT8" s="9" t="s">
         <v>614</v>
       </c>
       <c r="AU8" s="9" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="AW8" s="9" t="s">
         <v>614</v>
       </c>
       <c r="AX8" s="9" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="AY8" s="74"/>
       <c r="AZ8" s="9"/>
@@ -9176,10 +9235,10 @@
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>421</v>
@@ -9187,91 +9246,91 @@
       <c r="D9" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E9" s="95" t="s">
-        <v>689</v>
+      <c r="E9" s="94" t="s">
+        <v>690</v>
       </c>
       <c r="F9" s="9">
         <v>1100</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>236</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P9" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U9" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V9" s="10" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="X9" s="10" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="Y9" s="10" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="Z9" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA9" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB9" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC9" s="9"/>
       <c r="AD9" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="69"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI9" s="9"/>
       <c r="AJ9" s="9" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="AK9" s="9"/>
       <c r="AL9" s="9"/>
@@ -9279,39 +9338,39 @@
       <c r="AN9" s="9"/>
       <c r="AO9" s="9"/>
       <c r="AP9" s="13" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="AQ9" s="9" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="AR9" s="9" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="AS9" s="9" t="s">
-        <v>826</v>
-      </c>
-      <c r="AT9" s="85" t="s">
+        <v>827</v>
+      </c>
+      <c r="AT9" s="84" t="s">
+        <v>692</v>
+      </c>
+      <c r="AU9" s="14" t="s">
+        <v>679</v>
+      </c>
+      <c r="AV9" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="AU9" s="14" t="s">
-        <v>678</v>
-      </c>
-      <c r="AV9" s="9" t="s">
-        <v>690</v>
-      </c>
-      <c r="AW9" s="85" t="s">
-        <v>691</v>
+      <c r="AW9" s="84" t="s">
+        <v>692</v>
       </c>
       <c r="AX9" s="9" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>421</v>
@@ -9319,91 +9378,91 @@
       <c r="D10" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="E10" s="95" t="s">
-        <v>689</v>
+      <c r="E10" s="94" t="s">
+        <v>690</v>
       </c>
       <c r="F10" s="9">
         <v>1100</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>236</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="P10" s="10" t="s">
         <v>254</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="W10" s="10" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="Y10" s="10" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="Z10" s="10" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="AA10" s="10" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="AB10" s="10" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="AC10" s="9"/>
       <c r="AD10" s="10" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="69"/>
       <c r="AG10" s="9"/>
       <c r="AH10" s="10" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="AI10" s="9"/>
       <c r="AJ10" s="9" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="AK10" s="9"/>
       <c r="AL10" s="15"/>
@@ -9411,31 +9470,31 @@
       <c r="AN10" s="15"/>
       <c r="AO10" s="15"/>
       <c r="AP10" s="70" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="AQ10" s="70" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="AR10" s="70" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="AS10" s="70" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="AT10" s="16" t="s">
+        <v>692</v>
+      </c>
+      <c r="AU10" s="17" t="s">
+        <v>679</v>
+      </c>
+      <c r="AV10" s="15" t="s">
         <v>691</v>
       </c>
-      <c r="AU10" s="17" t="s">
-        <v>678</v>
-      </c>
-      <c r="AV10" s="15" t="s">
-        <v>690</v>
-      </c>
       <c r="AW10" s="16" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="AX10" s="9" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature/GDE-9581 prepayment via paperclip for PIM Future BILAT
Added new test suite, keyword, and locator
Updated data set
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7079D984-173B-4598-9A7B-E10009F80FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2919FBF-59B2-4B50-84B0-188170615028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="2790" windowWidth="21600" windowHeight="11385" tabRatio="842" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PTY001_QuickPartyOnboarding" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="900">
   <si>
     <t>rowid</t>
   </si>
@@ -2729,6 +2729,12 @@
   </si>
   <si>
     <t>12-Jun-2023</t>
+  </si>
+  <si>
+    <t>07-Feb-2020</t>
+  </si>
+  <si>
+    <t>Principal Prepayment of $157,000AUD</t>
   </si>
 </sst>
 </file>
@@ -2741,7 +2747,7 @@
     <numFmt numFmtId="166" formatCode="00000"/>
     <numFmt numFmtId="167" formatCode="0.00000%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2856,6 +2862,12 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -2992,7 +3004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3279,6 +3291,9 @@
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4137,8 +4152,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4278,8 +4293,8 @@
   </sheetPr>
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4289,11 +4304,9 @@
     <col min="3" max="3" width="28.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.140625" style="2" bestFit="1" customWidth="1"/>
@@ -4539,6 +4552,58 @@
       <c r="AP2" s="24"/>
       <c r="AQ2" s="24"/>
     </row>
+    <row r="3" spans="1:43" s="73" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="96" t="s">
+        <v>689</v>
+      </c>
+      <c r="B3" s="96" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="84" t="s">
+        <v>864</v>
+      </c>
+      <c r="F3" s="84" t="s">
+        <v>898</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>899</v>
+      </c>
+      <c r="H3" s="84" t="s">
+        <v>866</v>
+      </c>
+      <c r="I3" s="99">
+        <v>157000</v>
+      </c>
+      <c r="J3" s="85" t="s">
+        <v>868</v>
+      </c>
+      <c r="K3" s="85" t="s">
+        <v>869</v>
+      </c>
+      <c r="L3" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="9">
+        <v>428.64</v>
+      </c>
+      <c r="N3" s="84" t="s">
+        <v>871</v>
+      </c>
+      <c r="O3" s="96" t="s">
+        <v>426</v>
+      </c>
+      <c r="P3" s="96" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q3" s="96" t="s">
+        <v>872</v>
+      </c>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="25"/>
+    </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="S4" s="97" t="s">
         <v>875</v>
@@ -4548,6 +4613,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -4560,7 +4626,7 @@
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feature/GDE-9583 addressed review points
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Deal_PIM_Future_BILAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\NewUATDeals_DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3BF82C-8A5E-41B1-9ADD-5012EA10C029}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52470BC0-5812-411C-9CC5-7160562B4521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="905" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="889">
   <si>
     <t>rowid</t>
   </si>
@@ -2699,6 +2699,9 @@
   </si>
   <si>
     <t xml:space="preserve">Update row 2 to </t>
+  </si>
+  <si>
+    <t>Increase_Actual_Amount</t>
   </si>
 </sst>
 </file>
@@ -4504,10 +4507,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4527,17 +4530,18 @@
     <col min="13" max="13" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="79" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="79" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -4583,32 +4587,35 @@
       <c r="O1" s="17" t="s">
         <v>879</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="93" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q1" s="27" t="s">
         <v>880</v>
       </c>
-      <c r="Q1" s="93" t="s">
+      <c r="R1" s="93" t="s">
         <v>850</v>
       </c>
-      <c r="R1" s="93" t="s">
+      <c r="S1" s="93" t="s">
         <v>851</v>
       </c>
-      <c r="S1" s="93" t="s">
+      <c r="T1" s="93" t="s">
         <v>605</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>882</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>660</v>
       </c>
-      <c r="V1" s="17" t="s">
+      <c r="W1" s="17" t="s">
         <v>661</v>
       </c>
-      <c r="W1" s="17" t="s">
+      <c r="X1" s="17" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78" t="s">
         <v>81</v>
       </c>
@@ -4647,7 +4654,7 @@
       <c r="N2" s="31"/>
       <c r="O2" s="31"/>
     </row>
-    <row r="3" spans="1:23" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="78" t="s">
         <v>680</v>
       </c>
@@ -4693,23 +4700,23 @@
       <c r="O3" s="78" t="s">
         <v>864</v>
       </c>
-      <c r="P3" s="90" t="s">
+      <c r="P3" s="78" t="s">
+        <v>875</v>
+      </c>
+      <c r="Q3" s="90" t="s">
         <v>881</v>
       </c>
-      <c r="Q3" s="98" t="s">
+      <c r="R3" s="98" t="s">
         <v>861</v>
       </c>
-      <c r="R3" s="98" t="s">
+      <c r="S3" s="98" t="s">
         <v>862</v>
       </c>
-      <c r="S3" s="102" t="s">
+      <c r="T3" s="102" t="s">
         <v>885</v>
       </c>
-      <c r="T3" s="78" t="s">
+      <c r="U3" s="78" t="s">
         <v>883</v>
-      </c>
-      <c r="U3" s="90" t="s">
-        <v>886</v>
       </c>
       <c r="V3" s="90" t="s">
         <v>886</v>
@@ -4717,14 +4724,18 @@
       <c r="W3" s="90" t="s">
         <v>886</v>
       </c>
+      <c r="X3" s="90" t="s">
+        <v>886</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="R4" s="85" t="s">
         <v>887</v>
       </c>
       <c r="S4" s="86" t="s">
         <v>864</v>
       </c>
+      <c r="T4" s="86"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>